<commit_message>
Polished Tests and set tests to run parallel
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kwazinkosizwane\eclipse-workspace\takealot-automation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B42ED3F-FED6-453F-BB7E-4040323AC67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF613DE3-40E4-4CDB-B4FE-B988C3419BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5616" yWindow="1728" windowWidth="17424" windowHeight="10212" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="registration form" sheetId="4" r:id="rId3"/>
     <sheet name="login form" sheetId="7" r:id="rId4"/>
     <sheet name="products" sheetId="5" r:id="rId5"/>
-    <sheet name="test execution" sheetId="6" r:id="rId6"/>
+    <sheet name="execution" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1691,7 +1691,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>